<commit_message>
Concept method for generating goal
statement slightly changed and note added
</commit_message>
<xml_diff>
--- a/concepts/Interpreted text to goal.xlsx
+++ b/concepts/Interpreted text to goal.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14895" windowHeight="7875"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14895" windowHeight="7875" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
-    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
-    <sheet name="Blad3" sheetId="3" r:id="rId3"/>
+    <sheet name="Move1" sheetId="1" r:id="rId1"/>
+    <sheet name="Move2" sheetId="2" r:id="rId2"/>
+    <sheet name="Take1" sheetId="3" r:id="rId3"/>
+    <sheet name="Take2" sheetId="4" r:id="rId4"/>
+    <sheet name="Pruning" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="127">
   <si>
     <t>move(basic_entity(the,object(ball,(-),white)),relative(inside,relative_entity(any,object(box,(-),(-)),relative(ontop,floor))))</t>
   </si>
@@ -220,6 +222,183 @@
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>objects[1] relation1 objects[3] Given objects[1] fullfill relation2 to objects objects[2]</t>
+  </si>
+  <si>
+    <t>white ball ontop floor Given white ball in box</t>
+  </si>
+  <si>
+    <t>Move</t>
+  </si>
+  <si>
+    <t>First child</t>
+  </si>
+  <si>
+    <t>Second child</t>
+  </si>
+  <si>
+    <t>Current state of object</t>
+  </si>
+  <si>
+    <t>Goal State of object</t>
+  </si>
+  <si>
+    <t>take(basic_entity(any,object(anyform,(-),blue)))</t>
+  </si>
+  <si>
+    <t>Take</t>
+  </si>
+  <si>
+    <t>anyform</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>Goal State of object DOES NOT EXIST</t>
+  </si>
+  <si>
+    <t>Take two boxes on the table</t>
+  </si>
+  <si>
+    <t>Take all boxes</t>
+  </si>
+  <si>
+    <t>IMPOSSIBLE!</t>
+  </si>
+  <si>
+    <t>blue object held by robot Given no constraints</t>
+  </si>
+  <si>
+    <t>A list of all "blue objects"</t>
+  </si>
+  <si>
+    <t>Remove all objects in objects[1] that does not fullfill the requirments from the "Current state branch" and thereafter remove objects[2].</t>
+  </si>
+  <si>
+    <t>A list containing only the robot</t>
+  </si>
+  <si>
+    <t>A held by R</t>
+  </si>
+  <si>
+    <t>B held by R</t>
+  </si>
+  <si>
+    <t>blue object held by robot</t>
+  </si>
+  <si>
+    <t>objects[1] relation1 objects[3]</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>take(relative_entity(the,object(anyform,(-),(-)),relative(ontop,relative_entity(the,object(anyform,(-),(-)),relative(ontop,basic_entity(the,object(table,(-),(-))))))))</t>
+  </si>
+  <si>
+    <t>move(basic_entity(all,object(ball,(-),(-))),relative(inside,basic_entity(any,object(ball,(-),(-)))))</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>Output:</t>
+  </si>
+  <si>
+    <t>B in A</t>
+  </si>
+  <si>
+    <t>Prun both, since a ball cannot be on second possition of a "inside" statement.</t>
+  </si>
+  <si>
+    <t>A list of all "objects"</t>
+  </si>
+  <si>
+    <t>A list containing all "tables"</t>
+  </si>
+  <si>
+    <t>A on C</t>
+  </si>
+  <si>
+    <t>B on C</t>
+  </si>
+  <si>
+    <t>A on D</t>
+  </si>
+  <si>
+    <t>B on D</t>
+  </si>
+  <si>
+    <t>D in C</t>
+  </si>
+  <si>
+    <t>B in F</t>
+  </si>
+  <si>
+    <t>A in B and B in F</t>
+  </si>
+  <si>
+    <t>D in B and B in F</t>
+  </si>
+  <si>
+    <t>D in C and C in E</t>
+  </si>
+  <si>
+    <t>D in C and C in F</t>
+  </si>
+  <si>
+    <t>objects[4] =</t>
+  </si>
+  <si>
+    <t>C on E</t>
+  </si>
+  <si>
+    <t>C on F</t>
+  </si>
+  <si>
+    <t>D on E</t>
+  </si>
+  <si>
+    <t>D on F</t>
+  </si>
+  <si>
+    <t>E on T</t>
+  </si>
+  <si>
+    <t>F on T</t>
+  </si>
+  <si>
+    <t>R hold A</t>
+  </si>
+  <si>
+    <t>R hold B</t>
+  </si>
+  <si>
+    <t>R hold A &amp; A on C &amp; C on E &amp; E on T</t>
+  </si>
+  <si>
+    <t>R hold A &amp; A on C &amp; C on F &amp; F on T</t>
+  </si>
+  <si>
+    <t>R hold A &amp; A on D &amp; D on E &amp; E on T</t>
+  </si>
+  <si>
+    <t>R hold A &amp; A on D &amp; D on F &amp; F on T</t>
+  </si>
+  <si>
+    <t>R hold B &amp; B on C &amp; C on E &amp; E on T</t>
+  </si>
+  <si>
+    <t>R hold B &amp; B on C &amp; C on F &amp; F on T</t>
+  </si>
+  <si>
+    <t>R hold B &amp; B on D &amp; D on E &amp; E on T</t>
+  </si>
+  <si>
+    <t>R hold B &amp; B on D &amp; D on F &amp; F on T</t>
   </si>
 </sst>
 </file>
@@ -264,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -286,6 +465,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,9 +765,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:R45"/>
+  <dimension ref="A2:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -898,10 +1080,10 @@
       </c>
     </row>
     <row r="41" spans="2:7">
-      <c r="D41" s="9" t="s">
+      <c r="D41" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="9"/>
+      <c r="E41" s="10"/>
       <c r="F41" s="8"/>
       <c r="G41" t="s">
         <v>67</v>
@@ -923,13 +1105,13 @@
         <v>58</v>
       </c>
       <c r="E43" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G43" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="2:7">
@@ -937,15 +1119,41 @@
         <v>59</v>
       </c>
       <c r="E44" t="s">
+        <v>61</v>
+      </c>
+      <c r="G44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7">
+      <c r="D45" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" t="s">
         <v>62</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G45" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="2:7">
-      <c r="G45" t="s">
+    <row r="46" spans="2:7">
+      <c r="G46" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="G47" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7">
+      <c r="G48" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7">
+      <c r="G49" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -959,21 +1167,998 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C2"/>
+  <dimension ref="A2:AE57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:31">
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
+    </row>
+    <row r="4" spans="1:31">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31">
+      <c r="A5" s="5"/>
+      <c r="P5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="1:31">
+      <c r="A6" s="5"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+    </row>
+    <row r="7" spans="1:31">
+      <c r="A7" s="5"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+    </row>
+    <row r="8" spans="1:31">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="9"/>
+      <c r="P8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+    </row>
+    <row r="9" spans="1:31">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="P9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+    </row>
+    <row r="10" spans="1:31">
+      <c r="A10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="K10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+    </row>
+    <row r="11" spans="1:31">
+      <c r="A11" s="9"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="K11" s="9"/>
+      <c r="P11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+    </row>
+    <row r="12" spans="1:31">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+    </row>
+    <row r="13" spans="1:31">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="9"/>
+    </row>
+    <row r="14" spans="1:31">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="H14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="9"/>
+    </row>
+    <row r="15" spans="1:31">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="R15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="9"/>
+      <c r="AC15" s="9"/>
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="9"/>
+    </row>
+    <row r="16" spans="1:31">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="I16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="9"/>
+    </row>
+    <row r="17" spans="1:31">
+      <c r="A17" s="5"/>
+      <c r="B17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="9"/>
+      <c r="AC17" s="9"/>
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="9"/>
+    </row>
+    <row r="18" spans="1:31">
+      <c r="A18" s="5"/>
+      <c r="B18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" s="9"/>
+      <c r="AB18" s="9"/>
+      <c r="AC18" s="9"/>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="9"/>
+    </row>
+    <row r="19" spans="1:31">
+      <c r="A19" s="5"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="9"/>
+      <c r="AC19" s="9"/>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="9"/>
+    </row>
+    <row r="20" spans="1:31">
+      <c r="A20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="5"/>
+      <c r="AC20" s="5"/>
+      <c r="AD20" s="5"/>
+      <c r="AE20" s="5"/>
+    </row>
+    <row r="21" spans="1:31">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="5"/>
+      <c r="AC21" s="5"/>
+      <c r="AD21" s="5"/>
+      <c r="AE21" s="5"/>
+    </row>
+    <row r="22" spans="1:31">
+      <c r="A22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5"/>
+      <c r="AC22" s="5"/>
+      <c r="AD22" s="5"/>
+      <c r="AE22" s="5"/>
+    </row>
+    <row r="23" spans="1:31">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+      <c r="AA23" s="9"/>
+      <c r="AB23" s="9"/>
+      <c r="AC23" s="5"/>
+      <c r="AD23" s="5"/>
+      <c r="AE23" s="5"/>
+    </row>
+    <row r="24" spans="1:31">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+      <c r="AA24" s="9"/>
+      <c r="AB24" s="9"/>
+      <c r="AC24" s="5"/>
+      <c r="AD24" s="5"/>
+      <c r="AE24" s="5"/>
+    </row>
+    <row r="25" spans="1:31">
+      <c r="A25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="5"/>
+      <c r="AB25" s="5"/>
+      <c r="AC25" s="5"/>
+      <c r="AD25" s="5"/>
+      <c r="AE25" s="5"/>
+    </row>
+    <row r="26" spans="1:31">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="5"/>
+      <c r="AB26" s="5"/>
+      <c r="AC26" s="5"/>
+      <c r="AD26" s="5"/>
+      <c r="AE26" s="5"/>
+    </row>
+    <row r="27" spans="1:31">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="5"/>
+      <c r="AC27" s="5"/>
+      <c r="AD27" s="5"/>
+      <c r="AE27" s="5"/>
+    </row>
+    <row r="28" spans="1:31">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="5"/>
+      <c r="AC28" s="5"/>
+      <c r="AD28" s="5"/>
+      <c r="AE28" s="5"/>
+    </row>
+    <row r="29" spans="1:31">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="5"/>
+      <c r="AB29" s="5"/>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="5"/>
+      <c r="AE29" s="5"/>
+    </row>
+    <row r="30" spans="1:31">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="W30" s="5"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="5"/>
+      <c r="AB30" s="5"/>
+      <c r="AC30" s="5"/>
+      <c r="AD30" s="5"/>
+      <c r="AE30" s="5"/>
+    </row>
+    <row r="31" spans="1:31">
+      <c r="A31" s="5"/>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31">
+      <c r="A32" s="5"/>
+      <c r="B32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="5"/>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="5"/>
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="G34" t="s">
+        <v>48</v>
+      </c>
+      <c r="H34" t="s">
+        <v>49</v>
+      </c>
+      <c r="P34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" s="5"/>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" s="5"/>
+      <c r="C36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" s="5"/>
+      <c r="D37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" s="5"/>
+      <c r="E38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39" s="5"/>
+      <c r="F39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" s="5"/>
+      <c r="F40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" s="5"/>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" s="5"/>
+      <c r="B42" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43" s="5"/>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" s="5"/>
+      <c r="C44" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" s="5"/>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" s="5"/>
+      <c r="D46" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="8"/>
+      <c r="F46" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" s="5"/>
+      <c r="D47" t="s">
+        <v>57</v>
+      </c>
+      <c r="F47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" s="5"/>
+      <c r="D48" t="s">
+        <v>58</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="5"/>
+      <c r="D49" t="s">
+        <v>59</v>
+      </c>
+      <c r="F49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="5"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="5"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="5"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="5"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="5"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="5"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="5"/>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -983,13 +2168,1331 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A2:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:18">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="5"/>
+      <c r="P5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="5"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="5"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="P8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="9"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="P9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="9"/>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="R10" s="9"/>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="9"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="K11" s="9"/>
+      <c r="P11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="9"/>
+      <c r="C12" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="Q14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="R14" s="9"/>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="R15" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="5"/>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="5"/>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" s="5"/>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" s="5"/>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" t="s">
+        <v>48</v>
+      </c>
+      <c r="H28" t="s">
+        <v>49</v>
+      </c>
+      <c r="P28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="5"/>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" s="5"/>
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="5"/>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" s="5"/>
+      <c r="E32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="5"/>
+      <c r="F33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="5"/>
+      <c r="F34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="5"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="5"/>
+      <c r="B36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="5"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="5"/>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="5"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="5"/>
+      <c r="D40" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40" s="8"/>
+      <c r="G40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="5"/>
+      <c r="D41" t="s">
+        <v>87</v>
+      </c>
+      <c r="G41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="5"/>
+      <c r="D42" t="s">
+        <v>88</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="5"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:R55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:18">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="5"/>
+      <c r="P5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="5"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="5"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="P8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="P9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="R10" s="9"/>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="9"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="K11" s="9"/>
+      <c r="P11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="Q12" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="G14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="Q14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="R14" s="9"/>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="R15" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="5"/>
+      <c r="B17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="5"/>
+      <c r="B18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="M18" t="s">
+        <v>5</v>
+      </c>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="P18" s="9"/>
+      <c r="R18" s="9"/>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="5"/>
+      <c r="B19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P19" s="2"/>
+      <c r="R19" s="9"/>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="5"/>
+      <c r="B20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="N20" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R20" s="9"/>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="5"/>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="5"/>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="5"/>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" s="5"/>
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="G35" t="s">
+        <v>48</v>
+      </c>
+      <c r="H35" t="s">
+        <v>49</v>
+      </c>
+      <c r="P35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" s="5"/>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" s="5"/>
+      <c r="C37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" s="5"/>
+      <c r="D38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39" s="5"/>
+      <c r="E39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" s="5"/>
+      <c r="F40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" s="5"/>
+      <c r="F41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" s="5"/>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43" s="5"/>
+      <c r="B43" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" s="5"/>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" s="5"/>
+      <c r="C45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" s="5"/>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" s="5"/>
+      <c r="C47" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="8"/>
+      <c r="H47" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" s="5"/>
+      <c r="C48" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48" t="s">
+        <v>100</v>
+      </c>
+      <c r="E48" t="s">
+        <v>111</v>
+      </c>
+      <c r="F48" t="s">
+        <v>115</v>
+      </c>
+      <c r="H48" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="5"/>
+      <c r="C49" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E49" t="s">
+        <v>112</v>
+      </c>
+      <c r="F49" t="s">
+        <v>116</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H49" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="5"/>
+      <c r="D50" t="s">
+        <v>101</v>
+      </c>
+      <c r="E50" t="s">
+        <v>113</v>
+      </c>
+      <c r="H50" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="D51" t="s">
+        <v>103</v>
+      </c>
+      <c r="E51" t="s">
+        <v>114</v>
+      </c>
+      <c r="H51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="H52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="H53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="H54" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="H55" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C47:F47"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added some supporting methods
</commit_message>
<xml_diff>
--- a/concepts/Interpreted text to goal.xlsx
+++ b/concepts/Interpreted text to goal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14895" windowHeight="7875" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14895" windowHeight="7875" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Move1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="129">
   <si>
     <t>move(basic_entity(the,object(ball,(-),white)),relative(inside,relative_entity(any,object(box,(-),(-)),relative(ontop,floor))))</t>
   </si>
@@ -399,6 +399,12 @@
   </si>
   <si>
     <t>R hold B &amp; B on D &amp; D on F &amp; F on T</t>
+  </si>
+  <si>
+    <t>this should probably be done when trying to apply the objects[x] on the relation</t>
+  </si>
+  <si>
+    <t>for example if relation is inside, all objecs in second element of statments that isn't a box is removed… with a tabu list.</t>
   </si>
 </sst>
 </file>
@@ -2682,7 +2688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -3453,10 +3459,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C9"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3492,6 +3498,16 @@
         <v>97</v>
       </c>
     </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Node ready for ALL
</commit_message>
<xml_diff>
--- a/concepts/Interpreted text to goal.xlsx
+++ b/concepts/Interpreted text to goal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14895" windowHeight="7875" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14895" windowHeight="7875" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Move1" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Take1" sheetId="3" r:id="rId3"/>
     <sheet name="Take2" sheetId="4" r:id="rId4"/>
     <sheet name="Pruning" sheetId="5" r:id="rId5"/>
+    <sheet name="All" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="140">
   <si>
     <t>move(basic_entity(the,object(ball,(-),white)),relative(inside,relative_entity(any,object(box,(-),(-)),relative(ontop,floor))))</t>
   </si>
@@ -405,6 +406,39 @@
   </si>
   <si>
     <t>for example if relation is inside, all objecs in second element of statments that isn't a box is removed… with a tabu list.</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>move(basic_entity(any,object(ball,(-),(-))),relative(inside,relative_entity(any,object(box,(-),(-)),relative(ontop,relative_entity(all,object(table,(-),(-)),relative(ontop,floor))))))</t>
+  </si>
+  <si>
+    <t>move(relative_entity(any,object(ball,(-),(-)),relative(inside,basic_entity(any,object(box,(-),(-))))),relative(ontop,relative_entity(all,object(table,(-),(-)),relative(ontop,floor))))</t>
+  </si>
+  <si>
+    <t>move(relative_entity(any,object(ball,(-),(-)),relative(inside,relative_entity(any,object(box,(-),(-)),relative(ontop,basic_entity(all,object(table,(-),(-))))))),relative(ontop,floor))</t>
+  </si>
+  <si>
+    <t>1 2 2 -1</t>
+  </si>
+  <si>
+    <t>1 2 2  Found_ALL! 1</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>1 2 2 3 3 4 4 4 3 4 4  Found_ALL! 5 5 6 6 6 5 6 6 -1</t>
+  </si>
+  <si>
+    <t>1 2 2  Found_ALL! 3 3 4 4 4 3 4 4 -1</t>
+  </si>
+  <si>
+    <t>1 2 2 3 3 4 4 4 3 4 4  Found_ALL! 2</t>
+  </si>
+  <si>
+    <t>Put a ball in a box on all tables on the floor</t>
   </si>
 </sst>
 </file>
@@ -449,7 +483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -477,17 +511,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -778,7 +811,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:R49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11:N14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1091,10 +1126,10 @@
       </c>
     </row>
     <row r="41" spans="2:7">
-      <c r="D41" s="10" t="s">
+      <c r="D41" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="10"/>
+      <c r="E41" s="11"/>
       <c r="F41" s="8"/>
       <c r="G41" t="s">
         <v>67</v>
@@ -3361,12 +3396,12 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47" s="5"/>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
       <c r="G47" s="8"/>
       <c r="H47" t="s">
         <v>67</v>
@@ -3466,9 +3501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -3516,4 +3549,283 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:19" s="12" customFormat="1"/>
+    <row r="2" spans="1:19">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="D5" s="10"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="E7" s="10"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="10"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O10" s="10"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="K11" s="10"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="10"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>129</v>
+      </c>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="S12" s="10"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S13" s="2"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="S18" s="12"/>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="S19" s="12"/>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="S20" s="12"/>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" t="s">
+        <v>136</v>
+      </c>
+      <c r="H22" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23" t="s">
+        <v>137</v>
+      </c>
+      <c r="H23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="A24" t="s">
+        <v>133</v>
+      </c>
+      <c r="H24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>